<commit_message>
edit, search, rating (completed)
</commit_message>
<xml_diff>
--- a/data/film.xlsx
+++ b/data/film.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,21 @@
           <t>year</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>watched</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>rate</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -456,24 +471,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Taxi Driver</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Oppenheimer</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2023</v>
+          <t>Interstellar</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20xx</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>★★★★★★★★★★ (10.0)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lil bit polishing on edit (unfinished = genre)
</commit_message>
<xml_diff>
--- a/data/film.xlsx
+++ b/data/film.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>genre</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>watched</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>rate</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>review</t>
         </is>
@@ -476,20 +481,56 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>20xx</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>★★★★★★★★★★ (10.0)</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>★★★★★ (5.0)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Very good! i like how cooper eventually meet his daughter again</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Taxi Driver</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>199x</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Action, Loneliness</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
little bit polishing (finished)
</commit_message>
<xml_diff>
--- a/data/film.xlsx
+++ b/data/film.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +472,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Interstellar</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>Look Back</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Action, Loneliness</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -497,7 +499,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Very good! i like how cooper eventually meet his daughter again</t>
+          <t>very sad, poor kid</t>
         </is>
       </c>
     </row>
@@ -507,30 +509,226 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Interstellar</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fiction, Space</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Taxi Driver</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>199x</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Action, Loneliness</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="C4" t="n">
+        <v>1999</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Loneliness</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Oppenheimer</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>History, Bomb, War</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>The Batman</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>action</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Batman</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Dawdaw</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>234</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Dawd, Ada, D, Wad</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sdawda</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>234</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Awdawd, Awda, Ad, Aw</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
i think it finished (really?)
</commit_message>
<xml_diff>
--- a/data/film.xlsx
+++ b/data/film.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,35 +436,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>genre</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>watched</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>rate</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>review</t>
         </is>
@@ -472,265 +477,39 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Look Back</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2023</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Interstellar</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Action, Loneliness</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Sad, Space</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>★★★★★ (5.0)</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>very sad, poor kid</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Interstellar</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Fiction, Space</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Taxi Driver</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1999</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Loneliness</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Oppenheimer</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>History, Bomb, War</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>The Batman</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Batman</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2022</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Action</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Dawdaw</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>234</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Dawd, Ada, D, Wad</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Sdawda</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>234</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Awdawd, Awda, Ad, Aw</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>very sad, i wish cooper didnt leave her daughter</t>
         </is>
       </c>
     </row>

</xml_diff>